<commit_message>
Maj diapo TOP véhicule
</commit_message>
<xml_diff>
--- a/03_Optimus/01_Documents Projet/01_Documents Organisation/04_Gantt_Intégration/Planning Intégration.xlsx
+++ b/03_Optimus/01_Documents Projet/01_Documents Organisation/04_Gantt_Intégration/Planning Intégration.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gameiro Nicolas\Documents\EPSA\Intergen\03_Optimus\03_Documents Projet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gameiro Nicolas\Documents\EPSA\Intergen\03_Optimus\01_Documents Projet\01_Documents Organisation\04_Gantt_Intégration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80BF3549-E755-49CD-952B-BA209D1BE2F7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A95A4F6-953E-4763-B063-2C56FC108D5B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" tabRatio="762" firstSheet="3" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" tabRatio="762" firstSheet="3" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vérifications" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="857" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="860" uniqueCount="386">
   <si>
     <t>Planning vérification Optimus</t>
   </si>
@@ -988,9 +988,6 @@
     <t>TOP Appro</t>
   </si>
   <si>
-    <t>Peinture PSEP</t>
-  </si>
-  <si>
     <t>AutoTech WE</t>
   </si>
   <si>
@@ -998,9 +995,6 @@
   </si>
   <si>
     <t>Soirée remerciement</t>
-  </si>
-  <si>
-    <t>Lancement Projet 2020</t>
   </si>
   <si>
     <t>Début essai</t>
@@ -1195,6 +1189,29 @@
   </si>
   <si>
     <t>Total Cumulé (Réel)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Lancement Projet 2020 - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <rFont val="Raleway"/>
+        <family val="2"/>
+      </rPr>
+      <t>Peinture PSEP</t>
+    </r>
+  </si>
+  <si>
+    <t>Envoie découpe réservoir</t>
+  </si>
+  <si>
+    <t>Soudure réservoir</t>
+  </si>
+  <si>
+    <t>Réponse Camping FS ATA</t>
   </si>
 </sst>
 </file>
@@ -1666,7 +1683,7 @@
       <alignment vertical="top"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="138">
+  <cellXfs count="139">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1888,6 +1905,18 @@
     <xf numFmtId="0" fontId="30" fillId="12" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1943,22 +1972,25 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="12" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="12" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1970,27 +2002,15 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3897,16 +3917,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A1" s="97" t="s">
+      <c r="A1" s="103" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="98"/>
-      <c r="C1" s="98"/>
-      <c r="D1" s="98"/>
-      <c r="E1" s="98"/>
-      <c r="F1" s="98"/>
-      <c r="G1" s="98"/>
-      <c r="H1" s="99"/>
+      <c r="B1" s="104"/>
+      <c r="C1" s="104"/>
+      <c r="D1" s="104"/>
+      <c r="E1" s="104"/>
+      <c r="F1" s="104"/>
+      <c r="G1" s="104"/>
+      <c r="H1" s="105"/>
       <c r="I1" s="9"/>
       <c r="J1" s="9"/>
       <c r="K1" s="9"/>
@@ -3971,7 +3991,7 @@
       <c r="Z2" s="9"/>
     </row>
     <row r="3" spans="1:26" ht="37.5">
-      <c r="A3" s="100" t="s">
+      <c r="A3" s="106" t="s">
         <v>32</v>
       </c>
       <c r="B3" s="11" t="s">
@@ -4013,7 +4033,7 @@
       <c r="Z3" s="9"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A4" s="101"/>
+      <c r="A4" s="107"/>
       <c r="B4" s="11" t="s">
         <v>63</v>
       </c>
@@ -4047,7 +4067,7 @@
       <c r="Z4" s="9"/>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A5" s="101"/>
+      <c r="A5" s="107"/>
       <c r="B5" s="11" t="s">
         <v>66</v>
       </c>
@@ -4081,7 +4101,7 @@
       <c r="Z5" s="9"/>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A6" s="101"/>
+      <c r="A6" s="107"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
@@ -4111,7 +4131,7 @@
       <c r="Z6" s="9"/>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A7" s="102"/>
+      <c r="A7" s="108"/>
       <c r="B7" s="11" t="s">
         <v>75</v>
       </c>
@@ -4149,7 +4169,7 @@
       <c r="Z7" s="9"/>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A8" s="103" t="s">
+      <c r="A8" s="109" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="15" t="s">
@@ -4189,7 +4209,7 @@
       <c r="Z8" s="9"/>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A9" s="101"/>
+      <c r="A9" s="107"/>
       <c r="B9" s="15" t="s">
         <v>107</v>
       </c>
@@ -4225,7 +4245,7 @@
       <c r="Z9" s="9"/>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A10" s="102"/>
+      <c r="A10" s="108"/>
       <c r="B10" s="15" t="s">
         <v>114</v>
       </c>
@@ -4261,7 +4281,7 @@
       <c r="Z10" s="9"/>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A11" s="104" t="s">
+      <c r="A11" s="110" t="s">
         <v>119</v>
       </c>
       <c r="B11" s="20" t="s">
@@ -4301,7 +4321,7 @@
       <c r="Z11" s="9"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A12" s="101"/>
+      <c r="A12" s="107"/>
       <c r="B12" s="20" t="s">
         <v>133</v>
       </c>
@@ -4337,7 +4357,7 @@
       <c r="Z12" s="9"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A13" s="101"/>
+      <c r="A13" s="107"/>
       <c r="B13" s="20" t="s">
         <v>135</v>
       </c>
@@ -4371,7 +4391,7 @@
       <c r="Z13" s="9"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A14" s="101"/>
+      <c r="A14" s="107"/>
       <c r="B14" s="20" t="s">
         <v>137</v>
       </c>
@@ -4405,7 +4425,7 @@
       <c r="Z14" s="9"/>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A15" s="102"/>
+      <c r="A15" s="108"/>
       <c r="B15" s="20"/>
       <c r="C15" s="20"/>
       <c r="D15" s="20"/>
@@ -4435,7 +4455,7 @@
       <c r="Z15" s="9"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A16" s="105" t="s">
+      <c r="A16" s="111" t="s">
         <v>139</v>
       </c>
       <c r="B16" s="23" t="s">
@@ -4477,7 +4497,7 @@
       <c r="Z16" s="9"/>
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A17" s="102"/>
+      <c r="A17" s="108"/>
       <c r="B17" s="23" t="s">
         <v>144</v>
       </c>
@@ -32073,10 +32093,10 @@
       <c r="A1" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="119" t="s">
+      <c r="B1" s="125" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="99"/>
+      <c r="C1" s="105"/>
       <c r="D1" s="34" t="s">
         <v>3</v>
       </c>
@@ -32293,7 +32313,7 @@
         <v>276</v>
       </c>
       <c r="C9" s="69" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="D9" s="62"/>
       <c r="E9" s="62" t="s">
@@ -32317,7 +32337,7 @@
       </c>
       <c r="B10" s="64"/>
       <c r="C10" s="62" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="D10" s="65">
         <v>8</v>
@@ -32329,7 +32349,7 @@
         <v>252</v>
       </c>
       <c r="G10" s="63" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="H10" s="63" t="s">
         <v>37</v>
@@ -32345,7 +32365,7 @@
       </c>
       <c r="B11" s="64"/>
       <c r="C11" s="62" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="D11" s="62">
         <v>9</v>
@@ -32371,7 +32391,7 @@
       </c>
       <c r="B12" s="63"/>
       <c r="C12" s="62" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D12" s="65"/>
       <c r="E12" s="62" t="s">
@@ -32397,7 +32417,7 @@
       </c>
       <c r="B13" s="71"/>
       <c r="C13" s="69" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="D13" s="72">
         <v>43776</v>
@@ -32423,7 +32443,7 @@
       </c>
       <c r="B14" s="64"/>
       <c r="C14" s="62" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="D14" s="65">
         <v>12</v>
@@ -32449,7 +32469,7 @@
       </c>
       <c r="B15" s="64"/>
       <c r="C15" s="62" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="D15" s="65">
         <v>13</v>
@@ -32477,7 +32497,7 @@
         <v>277</v>
       </c>
       <c r="C16" s="66" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D16" s="73">
         <v>7</v>
@@ -32503,7 +32523,7 @@
       </c>
       <c r="B17" s="74"/>
       <c r="C17" s="66" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D17" s="63">
         <v>15</v>
@@ -32954,9 +32974,9 @@
       <c r="A21" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="B21" s="115"/>
-      <c r="C21" s="116"/>
-      <c r="D21" s="116"/>
+      <c r="B21" s="121"/>
+      <c r="C21" s="122"/>
+      <c r="D21" s="122"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -32973,8 +32993,8 @@
   </sheetPr>
   <dimension ref="A1:T32"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="T10" sqref="T10"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1796875" defaultRowHeight="20" customHeight="1"/>
@@ -34326,27 +34346,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="24" customHeight="1">
-      <c r="A1" s="129" t="s">
+      <c r="A1" s="126" t="s">
         <v>298</v>
       </c>
-      <c r="B1" s="130"/>
-      <c r="C1" s="130"/>
-      <c r="D1" s="130"/>
-      <c r="E1" s="131"/>
-      <c r="F1" s="129" t="s">
+      <c r="B1" s="127"/>
+      <c r="C1" s="127"/>
+      <c r="D1" s="127"/>
+      <c r="E1" s="128"/>
+      <c r="F1" s="126" t="s">
         <v>299</v>
       </c>
-      <c r="G1" s="130"/>
-      <c r="H1" s="130"/>
-      <c r="I1" s="130"/>
-      <c r="J1" s="131"/>
-      <c r="K1" s="129" t="s">
+      <c r="G1" s="127"/>
+      <c r="H1" s="127"/>
+      <c r="I1" s="127"/>
+      <c r="J1" s="128"/>
+      <c r="K1" s="126" t="s">
         <v>300</v>
       </c>
-      <c r="L1" s="130"/>
-      <c r="M1" s="130"/>
-      <c r="N1" s="130"/>
-      <c r="O1" s="131"/>
+      <c r="L1" s="127"/>
+      <c r="M1" s="127"/>
+      <c r="N1" s="127"/>
+      <c r="O1" s="128"/>
     </row>
     <row r="2" spans="1:18" ht="25" customHeight="1">
       <c r="A2" s="52">
@@ -34376,12 +34396,12 @@
         <v>303</v>
       </c>
       <c r="M2" s="93" t="s">
-        <v>368</v>
-      </c>
-      <c r="N2" s="124">
+        <v>366</v>
+      </c>
+      <c r="N2" s="129">
         <v>14</v>
       </c>
-      <c r="O2" s="125"/>
+      <c r="O2" s="130"/>
     </row>
     <row r="3" spans="1:18" ht="25" customHeight="1">
       <c r="A3" s="52">
@@ -34409,10 +34429,10 @@
         <v>305</v>
       </c>
       <c r="M3" s="96" t="s">
-        <v>372</v>
-      </c>
-      <c r="N3" s="124"/>
-      <c r="O3" s="125"/>
+        <v>370</v>
+      </c>
+      <c r="N3" s="129"/>
+      <c r="O3" s="130"/>
     </row>
     <row r="4" spans="1:18" ht="25" customHeight="1">
       <c r="A4" s="52">
@@ -34442,8 +34462,8 @@
       <c r="M4" s="95" t="s">
         <v>308</v>
       </c>
-      <c r="N4" s="124"/>
-      <c r="O4" s="125"/>
+      <c r="N4" s="129"/>
+      <c r="O4" s="130"/>
     </row>
     <row r="5" spans="1:18" ht="25" customHeight="1">
       <c r="A5" s="52">
@@ -34453,10 +34473,10 @@
         <v>303</v>
       </c>
       <c r="C5" s="48"/>
-      <c r="D5" s="120">
+      <c r="D5" s="131">
         <v>6</v>
       </c>
-      <c r="E5" s="121"/>
+      <c r="E5" s="132"/>
       <c r="F5" s="53">
         <v>4</v>
       </c>
@@ -34464,12 +34484,12 @@
         <v>303</v>
       </c>
       <c r="H5" s="48" t="s">
-        <v>360</v>
-      </c>
-      <c r="I5" s="120">
+        <v>358</v>
+      </c>
+      <c r="I5" s="131">
         <v>10</v>
       </c>
-      <c r="J5" s="121"/>
+      <c r="J5" s="132"/>
       <c r="K5" s="52">
         <v>4</v>
       </c>
@@ -34477,8 +34497,8 @@
         <v>309</v>
       </c>
       <c r="M5" s="57"/>
-      <c r="N5" s="124"/>
-      <c r="O5" s="125"/>
+      <c r="N5" s="129"/>
+      <c r="O5" s="130"/>
     </row>
     <row r="6" spans="1:18" ht="25" customHeight="1">
       <c r="A6" s="52">
@@ -34499,7 +34519,7 @@
         <v>305</v>
       </c>
       <c r="H6" s="48" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="I6" s="49"/>
       <c r="J6" s="50"/>
@@ -34510,8 +34530,8 @@
         <v>301</v>
       </c>
       <c r="M6" s="57"/>
-      <c r="N6" s="124"/>
-      <c r="O6" s="125"/>
+      <c r="N6" s="129"/>
+      <c r="O6" s="130"/>
     </row>
     <row r="7" spans="1:18" ht="25" customHeight="1">
       <c r="A7" s="52">
@@ -34532,7 +34552,7 @@
         <v>305</v>
       </c>
       <c r="H7" s="48" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="I7" s="49"/>
       <c r="J7" s="50"/>
@@ -34543,8 +34563,8 @@
         <v>304</v>
       </c>
       <c r="M7" s="54"/>
-      <c r="N7" s="122"/>
-      <c r="O7" s="123"/>
+      <c r="N7" s="136"/>
+      <c r="O7" s="137"/>
       <c r="Q7" s="40" t="s">
         <v>312</v>
       </c>
@@ -34571,7 +34591,7 @@
         <v>309</v>
       </c>
       <c r="H8" s="48" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="I8" s="49"/>
       <c r="J8" s="50"/>
@@ -34582,9 +34602,9 @@
         <v>307</v>
       </c>
       <c r="M8" s="54"/>
-      <c r="N8" s="122"/>
-      <c r="O8" s="123"/>
-      <c r="Q8" s="133" t="s">
+      <c r="N8" s="136"/>
+      <c r="O8" s="137"/>
+      <c r="Q8" s="98" t="s">
         <v>306</v>
       </c>
       <c r="R8" s="41">
@@ -34607,8 +34627,8 @@
       <c r="G9" s="46" t="s">
         <v>301</v>
       </c>
-      <c r="H9" s="132" t="s">
-        <v>378</v>
+      <c r="H9" s="97" t="s">
+        <v>376</v>
       </c>
       <c r="I9" s="49"/>
       <c r="J9" s="50"/>
@@ -34619,11 +34639,11 @@
         <v>303</v>
       </c>
       <c r="M9" s="48"/>
-      <c r="N9" s="120">
+      <c r="N9" s="131">
         <v>15</v>
       </c>
-      <c r="O9" s="121"/>
-      <c r="Q9" s="133" t="s">
+      <c r="O9" s="132"/>
+      <c r="Q9" s="98" t="s">
         <v>313</v>
       </c>
       <c r="R9" s="41">
@@ -34658,9 +34678,9 @@
         <v>305</v>
       </c>
       <c r="M10" s="48"/>
-      <c r="N10" s="120"/>
-      <c r="O10" s="121"/>
-      <c r="Q10" s="133" t="s">
+      <c r="N10" s="131"/>
+      <c r="O10" s="132"/>
+      <c r="Q10" s="98" t="s">
         <v>315</v>
       </c>
       <c r="R10" s="41">
@@ -34684,7 +34704,7 @@
         <v>307</v>
       </c>
       <c r="H11" s="54" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="I11" s="55"/>
       <c r="J11" s="56"/>
@@ -34697,9 +34717,9 @@
       <c r="M11" s="94" t="s">
         <v>316</v>
       </c>
-      <c r="N11" s="120"/>
-      <c r="O11" s="121"/>
-      <c r="Q11" s="133" t="s">
+      <c r="N11" s="131"/>
+      <c r="O11" s="132"/>
+      <c r="Q11" s="98" t="s">
         <v>317</v>
       </c>
       <c r="R11" s="41">
@@ -34714,10 +34734,10 @@
         <v>303</v>
       </c>
       <c r="C12" s="48"/>
-      <c r="D12" s="120">
+      <c r="D12" s="131">
         <v>7</v>
       </c>
-      <c r="E12" s="121"/>
+      <c r="E12" s="132"/>
       <c r="F12" s="53">
         <v>11</v>
       </c>
@@ -34725,12 +34745,12 @@
         <v>303</v>
       </c>
       <c r="H12" s="48" t="s">
-        <v>373</v>
-      </c>
-      <c r="I12" s="120">
+        <v>371</v>
+      </c>
+      <c r="I12" s="131">
         <v>11</v>
       </c>
-      <c r="J12" s="121"/>
+      <c r="J12" s="132"/>
       <c r="K12" s="52">
         <v>11</v>
       </c>
@@ -34738,10 +34758,10 @@
         <v>309</v>
       </c>
       <c r="M12" s="48"/>
-      <c r="N12" s="120"/>
-      <c r="O12" s="121"/>
-      <c r="Q12" s="133" t="s">
-        <v>319</v>
+      <c r="N12" s="131"/>
+      <c r="O12" s="132"/>
+      <c r="Q12" s="98" t="s">
+        <v>318</v>
       </c>
       <c r="R12" s="42"/>
     </row>
@@ -34761,8 +34781,8 @@
       <c r="G13" s="46" t="s">
         <v>305</v>
       </c>
-      <c r="H13" s="93" t="s">
-        <v>318</v>
+      <c r="H13" s="57" t="s">
+        <v>374</v>
       </c>
       <c r="I13" s="58"/>
       <c r="J13" s="59"/>
@@ -34772,11 +34792,13 @@
       <c r="L13" s="46" t="s">
         <v>301</v>
       </c>
-      <c r="M13" s="48"/>
-      <c r="N13" s="120"/>
-      <c r="O13" s="121"/>
-      <c r="Q13" s="133" t="s">
-        <v>320</v>
+      <c r="M13" s="138" t="s">
+        <v>385</v>
+      </c>
+      <c r="N13" s="131"/>
+      <c r="O13" s="132"/>
+      <c r="Q13" s="98" t="s">
+        <v>319</v>
       </c>
       <c r="R13" s="41">
         <v>41910</v>
@@ -34790,7 +34812,7 @@
         <v>305</v>
       </c>
       <c r="C14" s="94" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D14" s="49"/>
       <c r="E14" s="50"/>
@@ -34801,7 +34823,7 @@
         <v>305</v>
       </c>
       <c r="H14" s="57" t="s">
-        <v>322</v>
+        <v>382</v>
       </c>
       <c r="I14" s="58"/>
       <c r="J14" s="59"/>
@@ -34812,12 +34834,12 @@
         <v>304</v>
       </c>
       <c r="M14" s="54" t="s">
-        <v>323</v>
-      </c>
-      <c r="N14" s="122"/>
-      <c r="O14" s="123"/>
-      <c r="Q14" s="133" t="s">
-        <v>324</v>
+        <v>321</v>
+      </c>
+      <c r="N14" s="136"/>
+      <c r="O14" s="137"/>
+      <c r="Q14" s="98" t="s">
+        <v>322</v>
       </c>
       <c r="R14" s="41">
         <v>41920</v>
@@ -34831,7 +34853,7 @@
         <v>309</v>
       </c>
       <c r="C15" s="48" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D15" s="49"/>
       <c r="E15" s="50"/>
@@ -34842,7 +34864,7 @@
         <v>309</v>
       </c>
       <c r="H15" s="57" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="I15" s="58"/>
       <c r="J15" s="59"/>
@@ -34853,10 +34875,10 @@
         <v>307</v>
       </c>
       <c r="M15" s="54"/>
-      <c r="N15" s="122"/>
-      <c r="O15" s="123"/>
-      <c r="Q15" s="133" t="s">
-        <v>327</v>
+      <c r="N15" s="136"/>
+      <c r="O15" s="137"/>
+      <c r="Q15" s="98" t="s">
+        <v>325</v>
       </c>
       <c r="R15" s="41">
         <v>41955</v>
@@ -34879,7 +34901,7 @@
         <v>301</v>
       </c>
       <c r="H16" s="95" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="I16" s="58"/>
       <c r="J16" s="59"/>
@@ -34890,11 +34912,11 @@
         <v>303</v>
       </c>
       <c r="M16" s="48"/>
-      <c r="N16" s="120">
+      <c r="N16" s="131">
         <v>16</v>
       </c>
-      <c r="O16" s="121"/>
-      <c r="Q16" s="133" t="s">
+      <c r="O16" s="132"/>
+      <c r="Q16" s="98" t="s">
         <v>311</v>
       </c>
       <c r="R16" s="41">
@@ -34918,7 +34940,7 @@
         <v>304</v>
       </c>
       <c r="H17" s="92" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="I17" s="55"/>
       <c r="J17" s="56"/>
@@ -34929,9 +34951,9 @@
         <v>305</v>
       </c>
       <c r="M17" s="48"/>
-      <c r="N17" s="120"/>
-      <c r="O17" s="121"/>
-      <c r="Q17" s="133" t="s">
+      <c r="N17" s="131"/>
+      <c r="O17" s="132"/>
+      <c r="Q17" s="98" t="s">
         <v>310</v>
       </c>
       <c r="R17" s="41">
@@ -34955,7 +34977,7 @@
         <v>307</v>
       </c>
       <c r="H18" s="54" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="I18" s="55"/>
       <c r="J18" s="56"/>
@@ -34966,10 +34988,10 @@
         <v>305</v>
       </c>
       <c r="M18" s="48"/>
-      <c r="N18" s="120"/>
-      <c r="O18" s="121"/>
-      <c r="Q18" s="134" t="s">
-        <v>328</v>
+      <c r="N18" s="131"/>
+      <c r="O18" s="132"/>
+      <c r="Q18" s="99" t="s">
+        <v>326</v>
       </c>
       <c r="R18" s="41">
         <v>42078</v>
@@ -34983,23 +35005,25 @@
         <v>303</v>
       </c>
       <c r="C19" s="48" t="s">
-        <v>329</v>
-      </c>
-      <c r="D19" s="120">
+        <v>327</v>
+      </c>
+      <c r="D19" s="131">
         <v>8</v>
       </c>
-      <c r="E19" s="121"/>
+      <c r="E19" s="132"/>
       <c r="F19" s="53">
         <v>18</v>
       </c>
       <c r="G19" s="46" t="s">
         <v>303</v>
       </c>
-      <c r="H19" s="48"/>
-      <c r="I19" s="120">
+      <c r="H19" s="48" t="s">
+        <v>383</v>
+      </c>
+      <c r="I19" s="131">
         <v>12</v>
       </c>
-      <c r="J19" s="121"/>
+      <c r="J19" s="132"/>
       <c r="K19" s="52">
         <v>18</v>
       </c>
@@ -35007,16 +35031,16 @@
         <v>309</v>
       </c>
       <c r="M19" s="48"/>
-      <c r="N19" s="120"/>
-      <c r="O19" s="121"/>
-      <c r="Q19" s="134" t="s">
+      <c r="N19" s="131"/>
+      <c r="O19" s="132"/>
+      <c r="Q19" s="99" t="s">
         <v>308</v>
       </c>
       <c r="R19" s="41">
         <v>42097</v>
       </c>
       <c r="S19" s="44" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="T19" s="45">
         <v>42095</v>
@@ -35030,7 +35054,7 @@
         <v>305</v>
       </c>
       <c r="C20" s="48" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D20" s="49"/>
       <c r="E20" s="50"/>
@@ -35041,7 +35065,7 @@
         <v>305</v>
       </c>
       <c r="H20" s="48" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="I20" s="49"/>
       <c r="J20" s="50"/>
@@ -35052,10 +35076,10 @@
         <v>301</v>
       </c>
       <c r="M20" s="48"/>
-      <c r="N20" s="120"/>
-      <c r="O20" s="121"/>
-      <c r="Q20" s="134" t="s">
-        <v>332</v>
+      <c r="N20" s="131"/>
+      <c r="O20" s="132"/>
+      <c r="Q20" s="99" t="s">
+        <v>330</v>
       </c>
       <c r="R20" s="41">
         <v>42104</v>
@@ -35069,7 +35093,7 @@
         <v>305</v>
       </c>
       <c r="C21" s="48" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D21" s="49"/>
       <c r="E21" s="50"/>
@@ -35089,10 +35113,10 @@
         <v>304</v>
       </c>
       <c r="M21" s="54"/>
-      <c r="N21" s="122"/>
-      <c r="O21" s="123"/>
-      <c r="Q21" s="134" t="s">
-        <v>334</v>
+      <c r="N21" s="136"/>
+      <c r="O21" s="137"/>
+      <c r="Q21" s="99" t="s">
+        <v>332</v>
       </c>
       <c r="R21" s="41">
         <v>42166</v>
@@ -35106,7 +35130,7 @@
         <v>309</v>
       </c>
       <c r="C22" s="48" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="D22" s="49"/>
       <c r="E22" s="50"/>
@@ -35117,7 +35141,7 @@
         <v>309</v>
       </c>
       <c r="H22" s="48" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="I22" s="49"/>
       <c r="J22" s="50"/>
@@ -35128,13 +35152,13 @@
         <v>307</v>
       </c>
       <c r="M22" s="54"/>
-      <c r="N22" s="122"/>
-      <c r="O22" s="123"/>
-      <c r="Q22" s="134" t="s">
-        <v>336</v>
+      <c r="N22" s="136"/>
+      <c r="O22" s="137"/>
+      <c r="Q22" s="99" t="s">
+        <v>334</v>
       </c>
       <c r="R22" s="42" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="23" spans="1:20" ht="25" customHeight="1">
@@ -35145,7 +35169,7 @@
         <v>301</v>
       </c>
       <c r="C23" s="48" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D23" s="49"/>
       <c r="E23" s="50"/>
@@ -35156,7 +35180,7 @@
         <v>301</v>
       </c>
       <c r="H23" s="48" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="I23" s="49"/>
       <c r="J23" s="50"/>
@@ -35167,10 +35191,10 @@
         <v>303</v>
       </c>
       <c r="M23" s="48"/>
-      <c r="N23" s="120">
+      <c r="N23" s="131">
         <v>17</v>
       </c>
-      <c r="O23" s="121"/>
+      <c r="O23" s="132"/>
     </row>
     <row r="24" spans="1:20" ht="25" customHeight="1">
       <c r="A24" s="52">
@@ -35189,7 +35213,7 @@
         <v>304</v>
       </c>
       <c r="H24" s="54" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="I24" s="55"/>
       <c r="J24" s="56"/>
@@ -35200,8 +35224,8 @@
         <v>305</v>
       </c>
       <c r="M24" s="48"/>
-      <c r="N24" s="120"/>
-      <c r="O24" s="121"/>
+      <c r="N24" s="131"/>
+      <c r="O24" s="132"/>
     </row>
     <row r="25" spans="1:20" ht="25" customHeight="1">
       <c r="A25" s="52">
@@ -35220,7 +35244,7 @@
         <v>307</v>
       </c>
       <c r="H25" s="54" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="I25" s="55"/>
       <c r="J25" s="56"/>
@@ -35231,8 +35255,8 @@
         <v>305</v>
       </c>
       <c r="M25" s="48"/>
-      <c r="N25" s="120"/>
-      <c r="O25" s="121"/>
+      <c r="N25" s="131"/>
+      <c r="O25" s="132"/>
     </row>
     <row r="26" spans="1:20" ht="25" customHeight="1">
       <c r="A26" s="52">
@@ -35242,23 +35266,25 @@
         <v>303</v>
       </c>
       <c r="C26" s="93" t="s">
-        <v>339</v>
-      </c>
-      <c r="D26" s="124">
+        <v>337</v>
+      </c>
+      <c r="D26" s="129">
         <v>9</v>
       </c>
-      <c r="E26" s="125"/>
+      <c r="E26" s="130"/>
       <c r="F26" s="53">
         <v>25</v>
       </c>
       <c r="G26" s="46" t="s">
         <v>303</v>
       </c>
-      <c r="H26" s="48"/>
-      <c r="I26" s="120">
+      <c r="H26" s="48" t="s">
+        <v>384</v>
+      </c>
+      <c r="I26" s="131">
         <v>13</v>
       </c>
-      <c r="J26" s="121"/>
+      <c r="J26" s="132"/>
       <c r="K26" s="52">
         <v>25</v>
       </c>
@@ -35266,8 +35292,8 @@
         <v>309</v>
       </c>
       <c r="M26" s="48"/>
-      <c r="N26" s="120"/>
-      <c r="O26" s="121"/>
+      <c r="N26" s="131"/>
+      <c r="O26" s="132"/>
     </row>
     <row r="27" spans="1:20" ht="25" customHeight="1">
       <c r="A27" s="52">
@@ -35285,9 +35311,7 @@
       <c r="G27" s="46" t="s">
         <v>305</v>
       </c>
-      <c r="H27" s="48" t="s">
-        <v>377</v>
-      </c>
+      <c r="H27" s="48"/>
       <c r="I27" s="49"/>
       <c r="J27" s="50"/>
       <c r="K27" s="52">
@@ -35297,8 +35321,8 @@
         <v>301</v>
       </c>
       <c r="M27" s="48"/>
-      <c r="N27" s="120"/>
-      <c r="O27" s="121"/>
+      <c r="N27" s="131"/>
+      <c r="O27" s="132"/>
     </row>
     <row r="28" spans="1:20" ht="25" customHeight="1">
       <c r="A28" s="52">
@@ -35308,7 +35332,7 @@
         <v>305</v>
       </c>
       <c r="C28" s="57" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="D28" s="58"/>
       <c r="E28" s="59"/>
@@ -35328,8 +35352,8 @@
         <v>304</v>
       </c>
       <c r="M28" s="54"/>
-      <c r="N28" s="122"/>
-      <c r="O28" s="123"/>
+      <c r="N28" s="136"/>
+      <c r="O28" s="137"/>
     </row>
     <row r="29" spans="1:20" ht="25" customHeight="1">
       <c r="A29" s="52">
@@ -35339,7 +35363,7 @@
         <v>309</v>
       </c>
       <c r="C29" s="57" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="D29" s="58"/>
       <c r="E29" s="59"/>
@@ -35350,7 +35374,7 @@
         <v>309</v>
       </c>
       <c r="H29" s="48" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="I29" s="49"/>
       <c r="J29" s="50"/>
@@ -35361,8 +35385,8 @@
         <v>307</v>
       </c>
       <c r="M29" s="54"/>
-      <c r="N29" s="122"/>
-      <c r="O29" s="123"/>
+      <c r="N29" s="136"/>
+      <c r="O29" s="137"/>
     </row>
     <row r="30" spans="1:20" ht="25" customHeight="1">
       <c r="A30" s="51"/>
@@ -35386,10 +35410,10 @@
         <v>303</v>
       </c>
       <c r="M30" s="48"/>
-      <c r="N30" s="120">
+      <c r="N30" s="131">
         <v>18</v>
       </c>
-      <c r="O30" s="121"/>
+      <c r="O30" s="132"/>
     </row>
     <row r="31" spans="1:20" ht="25" customHeight="1">
       <c r="A31" s="51"/>
@@ -35404,7 +35428,7 @@
         <v>304</v>
       </c>
       <c r="H31" s="92" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="I31" s="55"/>
       <c r="J31" s="56"/>
@@ -35415,8 +35439,8 @@
         <v>305</v>
       </c>
       <c r="M31" s="48"/>
-      <c r="N31" s="120"/>
-      <c r="O31" s="121"/>
+      <c r="N31" s="131"/>
+      <c r="O31" s="132"/>
     </row>
     <row r="32" spans="1:20" ht="25" customHeight="1">
       <c r="A32" s="51"/>
@@ -35430,32 +35454,30 @@
       <c r="G32" s="46" t="s">
         <v>307</v>
       </c>
-      <c r="H32" s="54"/>
+      <c r="H32" s="54" t="s">
+        <v>375</v>
+      </c>
       <c r="I32" s="55"/>
       <c r="J32" s="56"/>
-      <c r="K32" s="126"/>
-      <c r="L32" s="127"/>
-      <c r="M32" s="127"/>
-      <c r="N32" s="127"/>
-      <c r="O32" s="128"/>
+      <c r="K32" s="133"/>
+      <c r="L32" s="134"/>
+      <c r="M32" s="134"/>
+      <c r="N32" s="134"/>
+      <c r="O32" s="135"/>
     </row>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="K1:O1"/>
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="K32:O32"/>
-    <mergeCell ref="N25:O25"/>
-    <mergeCell ref="N26:O26"/>
-    <mergeCell ref="N27:O27"/>
-    <mergeCell ref="N28:O28"/>
-    <mergeCell ref="N31:O31"/>
+    <mergeCell ref="N19:O19"/>
+    <mergeCell ref="N20:O20"/>
+    <mergeCell ref="N21:O21"/>
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="N24:O24"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="N8:O8"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="N9:O9"/>
     <mergeCell ref="N12:O12"/>
     <mergeCell ref="N23:O23"/>
     <mergeCell ref="D26:E26"/>
@@ -35472,17 +35494,21 @@
     <mergeCell ref="N17:O17"/>
     <mergeCell ref="N29:O29"/>
     <mergeCell ref="N18:O18"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="N7:O7"/>
-    <mergeCell ref="N8:O8"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="N9:O9"/>
-    <mergeCell ref="N19:O19"/>
-    <mergeCell ref="N20:O20"/>
-    <mergeCell ref="N21:O21"/>
-    <mergeCell ref="N22:O22"/>
-    <mergeCell ref="N24:O24"/>
+    <mergeCell ref="K32:O32"/>
+    <mergeCell ref="N25:O25"/>
+    <mergeCell ref="N26:O26"/>
+    <mergeCell ref="N27:O27"/>
+    <mergeCell ref="N28:O28"/>
+    <mergeCell ref="N31:O31"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="K1:O1"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="N5:O5"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -35498,7 +35524,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0728EA05-E77F-4C09-9E43-B2B05E54A2BF}">
   <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K42" sqref="K42"/>
     </sheetView>
   </sheetViews>
@@ -35513,498 +35539,498 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="13">
-      <c r="A1" s="135" t="s">
+      <c r="A1" s="100" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="135" t="s">
+      <c r="B1" s="100" t="s">
+        <v>378</v>
+      </c>
+      <c r="C1" s="100" t="s">
+        <v>379</v>
+      </c>
+      <c r="D1" s="100" t="s">
         <v>380</v>
       </c>
-      <c r="C1" s="135" t="s">
+      <c r="E1" s="100" t="s">
         <v>381</v>
       </c>
-      <c r="D1" s="135" t="s">
-        <v>382</v>
-      </c>
-      <c r="E1" s="135" t="s">
-        <v>383</v>
-      </c>
-      <c r="F1" s="135" t="s">
+      <c r="F1" s="100" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="136">
+      <c r="A2" s="101">
         <v>43540</v>
       </c>
-      <c r="B2" s="137">
+      <c r="B2" s="102">
         <v>20</v>
       </c>
-      <c r="C2" s="137">
+      <c r="C2" s="102">
         <f>B2</f>
         <v>20</v>
       </c>
-      <c r="D2" s="137">
+      <c r="D2" s="102">
         <v>10</v>
       </c>
-      <c r="E2" s="137">
+      <c r="E2" s="102">
         <f>D2</f>
         <v>10</v>
       </c>
-      <c r="F2" s="137"/>
+      <c r="F2" s="102"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="136">
+      <c r="A3" s="101">
         <v>43541</v>
       </c>
-      <c r="B3" s="137">
+      <c r="B3" s="102">
         <v>34</v>
       </c>
-      <c r="C3" s="137">
+      <c r="C3" s="102">
         <f>C2+B3</f>
         <v>54</v>
       </c>
-      <c r="D3" s="137">
+      <c r="D3" s="102">
         <v>15</v>
       </c>
-      <c r="E3" s="137">
+      <c r="E3" s="102">
         <f>E2+D3</f>
         <v>25</v>
       </c>
-      <c r="F3" s="137"/>
+      <c r="F3" s="102"/>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="136">
+      <c r="A4" s="101">
         <v>43542</v>
       </c>
-      <c r="B4" s="137">
+      <c r="B4" s="102">
         <v>45</v>
       </c>
-      <c r="C4" s="137">
+      <c r="C4" s="102">
         <f t="shared" ref="C4:C27" si="0">C3+B4</f>
         <v>99</v>
       </c>
-      <c r="D4" s="137">
+      <c r="D4" s="102">
         <v>35</v>
       </c>
-      <c r="E4" s="137">
+      <c r="E4" s="102">
         <f t="shared" ref="E4:E27" si="1">E3+D4</f>
         <v>60</v>
       </c>
-      <c r="F4" s="137"/>
+      <c r="F4" s="102"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="136">
+      <c r="A5" s="101">
         <v>43543</v>
       </c>
-      <c r="B5" s="137">
+      <c r="B5" s="102">
         <v>0</v>
       </c>
-      <c r="C5" s="137">
+      <c r="C5" s="102">
         <f t="shared" si="0"/>
         <v>99</v>
       </c>
-      <c r="D5" s="137"/>
-      <c r="E5" s="137">
+      <c r="D5" s="102"/>
+      <c r="E5" s="102">
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
-      <c r="F5" s="137"/>
+      <c r="F5" s="102"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="136">
+      <c r="A6" s="101">
         <v>43544</v>
       </c>
-      <c r="B6" s="137">
+      <c r="B6" s="102">
         <v>34</v>
       </c>
-      <c r="C6" s="137">
+      <c r="C6" s="102">
         <f t="shared" si="0"/>
         <v>133</v>
       </c>
-      <c r="D6" s="137"/>
-      <c r="E6" s="137">
+      <c r="D6" s="102"/>
+      <c r="E6" s="102">
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
-      <c r="F6" s="137"/>
+      <c r="F6" s="102"/>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="136">
+      <c r="A7" s="101">
         <v>43545</v>
       </c>
-      <c r="B7" s="137">
+      <c r="B7" s="102">
         <v>23</v>
       </c>
-      <c r="C7" s="137">
+      <c r="C7" s="102">
         <f t="shared" si="0"/>
         <v>156</v>
       </c>
-      <c r="D7" s="137"/>
-      <c r="E7" s="137">
+      <c r="D7" s="102"/>
+      <c r="E7" s="102">
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
-      <c r="F7" s="137"/>
+      <c r="F7" s="102"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="136">
+      <c r="A8" s="101">
         <v>43546</v>
       </c>
-      <c r="B8" s="137">
+      <c r="B8" s="102">
         <v>78</v>
       </c>
-      <c r="C8" s="137">
+      <c r="C8" s="102">
         <f t="shared" si="0"/>
         <v>234</v>
       </c>
-      <c r="D8" s="137"/>
-      <c r="E8" s="137">
+      <c r="D8" s="102"/>
+      <c r="E8" s="102">
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
-      <c r="F8" s="137"/>
+      <c r="F8" s="102"/>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="136">
+      <c r="A9" s="101">
         <v>43547</v>
       </c>
-      <c r="B9" s="137">
+      <c r="B9" s="102">
         <v>102</v>
       </c>
-      <c r="C9" s="137">
+      <c r="C9" s="102">
         <f t="shared" si="0"/>
         <v>336</v>
       </c>
-      <c r="D9" s="137"/>
-      <c r="E9" s="137">
+      <c r="D9" s="102"/>
+      <c r="E9" s="102">
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
-      <c r="F9" s="137"/>
+      <c r="F9" s="102"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="136">
+      <c r="A10" s="101">
         <v>43548</v>
       </c>
-      <c r="B10" s="137">
+      <c r="B10" s="102">
         <v>3</v>
       </c>
-      <c r="C10" s="137">
+      <c r="C10" s="102">
         <f t="shared" si="0"/>
         <v>339</v>
       </c>
-      <c r="D10" s="137"/>
-      <c r="E10" s="137">
+      <c r="D10" s="102"/>
+      <c r="E10" s="102">
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
-      <c r="F10" s="137"/>
+      <c r="F10" s="102"/>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="136">
+      <c r="A11" s="101">
         <v>43549</v>
       </c>
-      <c r="B11" s="137">
+      <c r="B11" s="102">
         <v>0</v>
       </c>
-      <c r="C11" s="137">
+      <c r="C11" s="102">
         <f t="shared" si="0"/>
         <v>339</v>
       </c>
-      <c r="D11" s="137"/>
-      <c r="E11" s="137">
+      <c r="D11" s="102"/>
+      <c r="E11" s="102">
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
-      <c r="F11" s="137"/>
+      <c r="F11" s="102"/>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="136">
+      <c r="A12" s="101">
         <v>43550</v>
       </c>
-      <c r="B12" s="137">
+      <c r="B12" s="102">
         <v>95</v>
       </c>
-      <c r="C12" s="137">
+      <c r="C12" s="102">
         <f t="shared" si="0"/>
         <v>434</v>
       </c>
-      <c r="D12" s="137"/>
-      <c r="E12" s="137">
+      <c r="D12" s="102"/>
+      <c r="E12" s="102">
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
-      <c r="F12" s="137"/>
+      <c r="F12" s="102"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="136">
+      <c r="A13" s="101">
         <v>43551</v>
       </c>
-      <c r="B13" s="137">
+      <c r="B13" s="102">
         <v>35</v>
       </c>
-      <c r="C13" s="137">
+      <c r="C13" s="102">
         <f t="shared" si="0"/>
         <v>469</v>
       </c>
-      <c r="D13" s="137"/>
-      <c r="E13" s="137">
+      <c r="D13" s="102"/>
+      <c r="E13" s="102">
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
-      <c r="F13" s="137"/>
+      <c r="F13" s="102"/>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="136">
+      <c r="A14" s="101">
         <v>43552</v>
       </c>
-      <c r="B14" s="137">
+      <c r="B14" s="102">
         <v>35</v>
       </c>
-      <c r="C14" s="137">
+      <c r="C14" s="102">
         <f t="shared" si="0"/>
         <v>504</v>
       </c>
-      <c r="D14" s="137"/>
-      <c r="E14" s="137">
+      <c r="D14" s="102"/>
+      <c r="E14" s="102">
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
-      <c r="F14" s="137"/>
+      <c r="F14" s="102"/>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="136">
+      <c r="A15" s="101">
         <v>43553</v>
       </c>
-      <c r="B15" s="137">
+      <c r="B15" s="102">
         <v>35</v>
       </c>
-      <c r="C15" s="137">
+      <c r="C15" s="102">
         <f t="shared" si="0"/>
         <v>539</v>
       </c>
-      <c r="D15" s="137"/>
-      <c r="E15" s="137">
+      <c r="D15" s="102"/>
+      <c r="E15" s="102">
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
-      <c r="F15" s="137"/>
+      <c r="F15" s="102"/>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="136">
+      <c r="A16" s="101">
         <v>43554</v>
       </c>
-      <c r="B16" s="137">
+      <c r="B16" s="102">
         <v>35</v>
       </c>
-      <c r="C16" s="137">
+      <c r="C16" s="102">
         <f t="shared" si="0"/>
         <v>574</v>
       </c>
-      <c r="D16" s="137"/>
-      <c r="E16" s="137">
+      <c r="D16" s="102"/>
+      <c r="E16" s="102">
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
-      <c r="F16" s="137"/>
+      <c r="F16" s="102"/>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="136">
+      <c r="A17" s="101">
         <v>43555</v>
       </c>
-      <c r="B17" s="137">
+      <c r="B17" s="102">
         <v>35</v>
       </c>
-      <c r="C17" s="137">
+      <c r="C17" s="102">
         <f t="shared" si="0"/>
         <v>609</v>
       </c>
-      <c r="D17" s="137"/>
-      <c r="E17" s="137">
+      <c r="D17" s="102"/>
+      <c r="E17" s="102">
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
-      <c r="F17" s="137"/>
+      <c r="F17" s="102"/>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="136">
+      <c r="A18" s="101">
         <v>43556</v>
       </c>
-      <c r="B18" s="137">
+      <c r="B18" s="102">
         <v>35</v>
       </c>
-      <c r="C18" s="137">
+      <c r="C18" s="102">
         <f t="shared" si="0"/>
         <v>644</v>
       </c>
-      <c r="D18" s="137"/>
-      <c r="E18" s="137">
+      <c r="D18" s="102"/>
+      <c r="E18" s="102">
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
-      <c r="F18" s="137"/>
+      <c r="F18" s="102"/>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="136">
+      <c r="A19" s="101">
         <v>43557</v>
       </c>
-      <c r="B19" s="137">
+      <c r="B19" s="102">
         <v>35</v>
       </c>
-      <c r="C19" s="137">
+      <c r="C19" s="102">
         <f t="shared" si="0"/>
         <v>679</v>
       </c>
-      <c r="D19" s="137"/>
-      <c r="E19" s="137">
+      <c r="D19" s="102"/>
+      <c r="E19" s="102">
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
-      <c r="F19" s="137"/>
+      <c r="F19" s="102"/>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="136">
+      <c r="A20" s="101">
         <v>43558</v>
       </c>
-      <c r="B20" s="137">
+      <c r="B20" s="102">
         <v>35</v>
       </c>
-      <c r="C20" s="137">
+      <c r="C20" s="102">
         <f t="shared" si="0"/>
         <v>714</v>
       </c>
-      <c r="D20" s="137"/>
-      <c r="E20" s="137">
+      <c r="D20" s="102"/>
+      <c r="E20" s="102">
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
-      <c r="F20" s="137"/>
+      <c r="F20" s="102"/>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="136">
+      <c r="A21" s="101">
         <v>43559</v>
       </c>
-      <c r="B21" s="137">
+      <c r="B21" s="102">
         <v>35</v>
       </c>
-      <c r="C21" s="137">
+      <c r="C21" s="102">
         <f t="shared" si="0"/>
         <v>749</v>
       </c>
-      <c r="D21" s="137"/>
-      <c r="E21" s="137">
+      <c r="D21" s="102"/>
+      <c r="E21" s="102">
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
-      <c r="F21" s="137"/>
+      <c r="F21" s="102"/>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="136">
+      <c r="A22" s="101">
         <v>43560</v>
       </c>
-      <c r="B22" s="137">
+      <c r="B22" s="102">
         <v>35</v>
       </c>
-      <c r="C22" s="137">
+      <c r="C22" s="102">
         <f t="shared" si="0"/>
         <v>784</v>
       </c>
-      <c r="D22" s="137"/>
-      <c r="E22" s="137">
+      <c r="D22" s="102"/>
+      <c r="E22" s="102">
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
-      <c r="F22" s="137"/>
+      <c r="F22" s="102"/>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="136">
+      <c r="A23" s="101">
         <v>43561</v>
       </c>
-      <c r="B23" s="137">
+      <c r="B23" s="102">
         <v>35</v>
       </c>
-      <c r="C23" s="137">
+      <c r="C23" s="102">
         <f t="shared" si="0"/>
         <v>819</v>
       </c>
-      <c r="D23" s="137"/>
-      <c r="E23" s="137">
+      <c r="D23" s="102"/>
+      <c r="E23" s="102">
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
-      <c r="F23" s="137"/>
+      <c r="F23" s="102"/>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="136">
+      <c r="A24" s="101">
         <v>43562</v>
       </c>
-      <c r="B24" s="137">
+      <c r="B24" s="102">
         <v>35</v>
       </c>
-      <c r="C24" s="137">
+      <c r="C24" s="102">
         <f t="shared" si="0"/>
         <v>854</v>
       </c>
-      <c r="D24" s="137"/>
-      <c r="E24" s="137">
+      <c r="D24" s="102"/>
+      <c r="E24" s="102">
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
-      <c r="F24" s="137"/>
+      <c r="F24" s="102"/>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="136">
+      <c r="A25" s="101">
         <v>43563</v>
       </c>
-      <c r="B25" s="137">
+      <c r="B25" s="102">
         <v>135</v>
       </c>
-      <c r="C25" s="137">
+      <c r="C25" s="102">
         <f t="shared" si="0"/>
         <v>989</v>
       </c>
-      <c r="D25" s="137"/>
-      <c r="E25" s="137">
+      <c r="D25" s="102"/>
+      <c r="E25" s="102">
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
-      <c r="F25" s="137"/>
+      <c r="F25" s="102"/>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="136">
+      <c r="A26" s="101">
         <v>43564</v>
       </c>
-      <c r="B26" s="137">
+      <c r="B26" s="102">
         <v>35</v>
       </c>
-      <c r="C26" s="137">
+      <c r="C26" s="102">
         <f t="shared" si="0"/>
         <v>1024</v>
       </c>
-      <c r="D26" s="137"/>
-      <c r="E26" s="137">
+      <c r="D26" s="102"/>
+      <c r="E26" s="102">
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
-      <c r="F26" s="137"/>
+      <c r="F26" s="102"/>
     </row>
     <row r="27" spans="1:6">
-      <c r="A27" s="136">
+      <c r="A27" s="101">
         <v>43565</v>
       </c>
-      <c r="B27" s="137">
+      <c r="B27" s="102">
         <v>35</v>
       </c>
-      <c r="C27" s="137">
+      <c r="C27" s="102">
         <f t="shared" si="0"/>
         <v>1059</v>
       </c>
-      <c r="D27" s="137"/>
-      <c r="E27" s="137">
+      <c r="D27" s="102"/>
+      <c r="E27" s="102">
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
-      <c r="F27" s="137"/>
+      <c r="F27" s="102"/>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="91"/>
@@ -36091,10 +36117,10 @@
       <c r="A1" s="79" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="108" t="s">
+      <c r="B1" s="114" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="109"/>
+      <c r="C1" s="115"/>
       <c r="D1" s="79" t="s">
         <v>3</v>
       </c>
@@ -36114,14 +36140,14 @@
         <v>8</v>
       </c>
       <c r="J1" s="87" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="13">
       <c r="A2" s="77">
         <v>1</v>
       </c>
-      <c r="B2" s="110" t="s">
+      <c r="B2" s="116" t="s">
         <v>12</v>
       </c>
       <c r="C2" s="81" t="s">
@@ -36151,7 +36177,7 @@
       <c r="A3" s="77">
         <v>2</v>
       </c>
-      <c r="B3" s="107"/>
+      <c r="B3" s="113"/>
       <c r="C3" s="82" t="s">
         <v>19</v>
       </c>
@@ -36181,7 +36207,7 @@
       <c r="A4" s="77">
         <v>3</v>
       </c>
-      <c r="B4" s="107"/>
+      <c r="B4" s="113"/>
       <c r="C4" s="81" t="s">
         <v>24</v>
       </c>
@@ -36211,7 +36237,7 @@
       <c r="A5" s="77">
         <v>4</v>
       </c>
-      <c r="B5" s="111" t="s">
+      <c r="B5" s="117" t="s">
         <v>35</v>
       </c>
       <c r="C5" s="82" t="s">
@@ -36241,7 +36267,7 @@
       <c r="A6" s="77">
         <v>5</v>
       </c>
-      <c r="B6" s="112"/>
+      <c r="B6" s="118"/>
       <c r="C6" s="82" t="s">
         <v>59</v>
       </c>
@@ -36268,7 +36294,7 @@
       <c r="A7" s="77">
         <v>6</v>
       </c>
-      <c r="B7" s="112"/>
+      <c r="B7" s="118"/>
       <c r="C7" s="82" t="s">
         <v>62</v>
       </c>
@@ -36295,7 +36321,7 @@
       <c r="A8" s="77">
         <v>7</v>
       </c>
-      <c r="B8" s="113"/>
+      <c r="B8" s="119"/>
       <c r="C8" s="82" t="s">
         <v>79</v>
       </c>
@@ -36325,7 +36351,7 @@
       <c r="A9" s="77">
         <v>8</v>
       </c>
-      <c r="B9" s="111" t="s">
+      <c r="B9" s="117" t="s">
         <v>85</v>
       </c>
       <c r="C9" s="82" t="s">
@@ -36335,7 +36361,7 @@
       <c r="E9" s="82" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="114">
+      <c r="F9" s="120">
         <v>1</v>
       </c>
       <c r="G9" s="82" t="s">
@@ -36355,7 +36381,7 @@
       <c r="A10" s="77">
         <v>9</v>
       </c>
-      <c r="B10" s="112"/>
+      <c r="B10" s="118"/>
       <c r="C10" s="82" t="s">
         <v>59</v>
       </c>
@@ -36365,7 +36391,7 @@
       <c r="E10" s="82" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="112"/>
+      <c r="F10" s="118"/>
       <c r="G10" s="82" t="s">
         <v>89</v>
       </c>
@@ -36380,7 +36406,7 @@
       <c r="A11" s="77">
         <v>10</v>
       </c>
-      <c r="B11" s="112"/>
+      <c r="B11" s="118"/>
       <c r="C11" s="82" t="s">
         <v>62</v>
       </c>
@@ -36390,7 +36416,7 @@
       <c r="E11" s="82" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="113"/>
+      <c r="F11" s="119"/>
       <c r="G11" s="82" t="s">
         <v>93</v>
       </c>
@@ -36405,7 +36431,7 @@
       <c r="A12" s="77">
         <v>11</v>
       </c>
-      <c r="B12" s="113"/>
+      <c r="B12" s="119"/>
       <c r="C12" s="82" t="s">
         <v>96</v>
       </c>
@@ -36435,7 +36461,7 @@
       <c r="A13" s="78">
         <v>12</v>
       </c>
-      <c r="B13" s="111" t="s">
+      <c r="B13" s="117" t="s">
         <v>99</v>
       </c>
       <c r="C13" s="82" t="s">
@@ -36465,7 +36491,7 @@
       <c r="A14" s="77">
         <v>13</v>
       </c>
-      <c r="B14" s="112"/>
+      <c r="B14" s="118"/>
       <c r="C14" s="82" t="s">
         <v>56</v>
       </c>
@@ -36473,7 +36499,7 @@
       <c r="E14" s="82" t="s">
         <v>15</v>
       </c>
-      <c r="F14" s="114">
+      <c r="F14" s="120">
         <v>1</v>
       </c>
       <c r="G14" s="82" t="s">
@@ -36490,7 +36516,7 @@
       <c r="A15" s="78">
         <v>14</v>
       </c>
-      <c r="B15" s="112"/>
+      <c r="B15" s="118"/>
       <c r="C15" s="82" t="s">
         <v>59</v>
       </c>
@@ -36500,7 +36526,7 @@
       <c r="E15" s="82" t="s">
         <v>15</v>
       </c>
-      <c r="F15" s="112"/>
+      <c r="F15" s="118"/>
       <c r="G15" s="82" t="s">
         <v>115</v>
       </c>
@@ -36518,7 +36544,7 @@
       <c r="A16" s="77">
         <v>15</v>
       </c>
-      <c r="B16" s="112"/>
+      <c r="B16" s="118"/>
       <c r="C16" s="82" t="s">
         <v>62</v>
       </c>
@@ -36528,7 +36554,7 @@
       <c r="E16" s="82" t="s">
         <v>15</v>
       </c>
-      <c r="F16" s="113"/>
+      <c r="F16" s="119"/>
       <c r="G16" s="82" t="s">
         <v>118</v>
       </c>
@@ -36543,7 +36569,7 @@
       <c r="A17" s="77">
         <v>16</v>
       </c>
-      <c r="B17" s="113"/>
+      <c r="B17" s="119"/>
       <c r="C17" s="82" t="s">
         <v>120</v>
       </c>
@@ -36580,27 +36606,27 @@
       <c r="A20" s="86" t="s">
         <v>117</v>
       </c>
-      <c r="B20" s="106" t="s">
+      <c r="B20" s="112" t="s">
         <v>130</v>
       </c>
-      <c r="C20" s="107"/>
-      <c r="D20" s="107"/>
-      <c r="E20" s="107"/>
+      <c r="C20" s="113"/>
+      <c r="D20" s="113"/>
+      <c r="E20" s="113"/>
     </row>
     <row r="21" spans="1:10" ht="15.75" customHeight="1">
-      <c r="B21" s="106" t="s">
+      <c r="B21" s="112" t="s">
         <v>131</v>
       </c>
-      <c r="C21" s="107"/>
-      <c r="D21" s="107"/>
-      <c r="E21" s="107"/>
+      <c r="C21" s="113"/>
+      <c r="D21" s="113"/>
+      <c r="E21" s="113"/>
       <c r="F21" s="84" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="15.75" customHeight="1">
       <c r="I23" s="87" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="J23" s="88">
         <v>43529</v>
@@ -36608,27 +36634,27 @@
     </row>
     <row r="24" spans="1:10" ht="15.75" customHeight="1">
       <c r="I24" s="87" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="15.75" customHeight="1">
       <c r="I25" s="87" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="15.75" customHeight="1">
       <c r="I26" s="87" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="15.75" customHeight="1">
       <c r="I27" s="87" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="15.75" customHeight="1">
       <c r="I28" s="87" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
   </sheetData>
@@ -36708,7 +36734,7 @@
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="90" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="5"/>
@@ -37040,9 +37066,9 @@
       <c r="A19" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="B19" s="115"/>
-      <c r="C19" s="116"/>
-      <c r="D19" s="116"/>
+      <c r="B19" s="121"/>
+      <c r="C19" s="122"/>
+      <c r="D19" s="122"/>
       <c r="F19" s="18" t="s">
         <v>123</v>
       </c>
@@ -37209,10 +37235,10 @@
       <c r="D5" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="E5" s="117" t="s">
+      <c r="E5" s="123" t="s">
         <v>152</v>
       </c>
-      <c r="F5" s="117" t="s">
+      <c r="F5" s="123" t="s">
         <v>160</v>
       </c>
       <c r="G5" s="3" t="s">
@@ -37238,8 +37264,8 @@
       <c r="D6" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="E6" s="102"/>
-      <c r="F6" s="102"/>
+      <c r="E6" s="108"/>
+      <c r="F6" s="108"/>
       <c r="G6" s="3" t="s">
         <v>37</v>
       </c>
@@ -37260,10 +37286,10 @@
       <c r="D7" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="E7" s="117" t="s">
+      <c r="E7" s="123" t="s">
         <v>165</v>
       </c>
-      <c r="F7" s="117" t="s">
+      <c r="F7" s="123" t="s">
         <v>160</v>
       </c>
       <c r="G7" s="3" t="s">
@@ -37286,8 +37312,8 @@
       <c r="D8" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="E8" s="102"/>
-      <c r="F8" s="102"/>
+      <c r="E8" s="108"/>
+      <c r="F8" s="108"/>
       <c r="G8" s="3" t="s">
         <v>37</v>
       </c>
@@ -37299,9 +37325,9 @@
       <c r="A10" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="B10" s="115"/>
-      <c r="C10" s="116"/>
-      <c r="D10" s="116"/>
+      <c r="B10" s="121"/>
+      <c r="C10" s="122"/>
+      <c r="D10" s="122"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -38024,9 +38050,9 @@
       <c r="A10" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="B10" s="115"/>
-      <c r="C10" s="116"/>
-      <c r="D10" s="116"/>
+      <c r="B10" s="121"/>
+      <c r="C10" s="122"/>
+      <c r="D10" s="122"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -38416,9 +38442,9 @@
       <c r="A10" s="30" t="s">
         <v>117</v>
       </c>
-      <c r="B10" s="118"/>
-      <c r="C10" s="116"/>
-      <c r="D10" s="116"/>
+      <c r="B10" s="124"/>
+      <c r="C10" s="122"/>
+      <c r="D10" s="122"/>
       <c r="E10" s="26"/>
       <c r="F10" s="26"/>
       <c r="G10" s="26"/>
@@ -65401,9 +65427,9 @@
       <c r="A12" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="B12" s="115"/>
-      <c r="C12" s="116"/>
-      <c r="D12" s="116"/>
+      <c r="B12" s="121"/>
+      <c r="C12" s="122"/>
+      <c r="D12" s="122"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -65604,9 +65630,9 @@
       <c r="A10" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="B10" s="115"/>
-      <c r="C10" s="116"/>
-      <c r="D10" s="116"/>
+      <c r="B10" s="121"/>
+      <c r="C10" s="122"/>
+      <c r="D10" s="122"/>
     </row>
     <row r="12" spans="1:9" ht="15.75" customHeight="1">
       <c r="D12" s="18" t="s">

</xml_diff>